<commit_message>
Improve boundary template handling and test workflow
- Enhanced template generation with better retry logic and timeout handling
- Updated sample file to remove Service Boundary Code data while preserving column structure
- Modified test_boundary_management_service to use uploaded FileStore ID for processing
- Added automatic template generation in test_upload_file for seamless workflow

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/sample/sample.xlsx
+++ b/sample/sample.xlsx
@@ -516,9 +516,6 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
-      <c r="H2" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="I2" s="2" t="s">
         <v>11</v>
       </c>
@@ -544,9 +541,6 @@
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
-      <c r="H3" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="I3" s="2" t="s">
         <v>13</v>
       </c>
@@ -570,9 +564,6 @@
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
-      <c r="H4" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="I4" s="2" t="s">
         <v>15</v>
       </c>
@@ -598,9 +589,6 @@
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
-      <c r="H5" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="I5" s="2" t="s">
         <v>17</v>
       </c>
@@ -628,9 +616,6 @@
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
-      <c r="H6" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="I6" s="2" t="s">
         <v>19</v>
       </c>
@@ -660,9 +645,6 @@
         <v>21</v>
       </c>
       <c r="G7" s="3"/>
-      <c r="H7" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="I7" s="2" t="s">
         <v>21</v>
       </c>
@@ -694,9 +676,6 @@
       <c r="G8" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="H8" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="I8" s="2" t="s">
         <v>23</v>
       </c>

</xml_diff>